<commit_message>
defs in different files
</commit_message>
<xml_diff>
--- a/resumes.xlsx
+++ b/resumes.xlsx
@@ -387,7 +387,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M231"/>
+  <dimension ref="A1:M239"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K56" sqref="K56"/>
@@ -17371,6 +17371,674 @@
         <v>43802</v>
       </c>
     </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Дмитрий</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>https://rabota.ua/cv/13672355</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>Киев</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>Эффективное управление коммерческой деятельностью предприятия;Глубокие знания и опыт работы на сырьевых рынках сельскохозяйственной продукции и на рынке FMCG (Food);Навыки стратегического планирования и построения эффективной системы продаж;Успешные кейсы по привлечению и построению эффективных взаимоотношений с ключевыми клиентами B2B и B2C;Опыт по подбору, обучению и управлению персоналом;</t>
+        </is>
+      </c>
+      <c r="I232" t="inlineStr">
+        <is>
+          <t>
+Заместитель коммерческого директорамай 2016 - настоящее время (3 года 8 мес)ПАО "Юрия" ТМ "Волошкове поле"FMCG
+				Обязанности:организация системы дистрибуции в нетрадиционных каналах сбыта (OOH, HoReCa, B2B, государственные и коммерческие закупки);организация и контроль работы менеджеров региональных структурных подразделений;проведение переговоров и привлечение ключевых клиентов;мониторинг рынка, конкурентный анализ;анализ и контроль дебиторской задолженности; Достижения:построение эффективной команды региональных менеджеров;внедрение  эффективной стратегии работы с государственными и коммерческими электронными тендерными площадками;привлечение к сотрудничеству ключевых клиентов, а именно: DCH, ДТЭК, Ferrex, Интерпайп, Glencore, Нибулон, HeidelbergСement, EVRAZ, Аскания-ПАК, КиевХлеб, Fornetti Kft, !Fest, FM Group, Пузата хата и ряд бюджетных организаций и учреждений на территории Украины;увеличение объемов реализации продукции в канале сбыта B2B на 40% в натуральном объеме и 90% в денежном объеме;Коммерческий директориюн 2015 - ноя 2015 (6 мес)Milkiland Ukraine, ООО "Первый Киевский молочный завод"FMCG
+				Обязанности:анализ продаж и разработка стратегических планов увеличения продаж;обеспечение выполнения плановых показателей;работа с дистрибьюторами бренда: проведение переговоров, постановка целей и задач, урегулирование вопросов дебиторской задолженности;контроль и обучение персонала коммерческой службы;координация работы коммерческой службы с прочими подразделениями компании;поиск и привлечение ключевых клиентов;анализ локального и национального рынков сбыта сыра и цельномолочной продукции, мониторинг работы конкурентов Достижения:увеличение показателей нумерической дистрибуции за счет привлечение к сотрудничеству региональных ритейлеров и дистрибьюторов;уменьшение дебиторской задолженности филиала  в 1,5 раза;эффективный кейс по реализации трейд-маркетинговой стратегии в оптовом канале сбыта;успешный вывод на рынок нового продукта компании;Руководитель отдела продаж (линейная розница, HoReCa, локальные сети)янв 2015 - июн 2015 (6 мес)Milkiland Ukraine, ООО "Первый Киевский молочный завод"FMCG
+				Обязанности:контроль за выполнением планов продаж;подбор, обучение и контроль персонала розничной торговой команды;определение стратегии и тактики сбыта продукции в канале сбыта;контроль за возвратом дебиторской задолженности; Достижения:выполнение плана продаж и поступления денежных средств;снижение уровня дебиторской задолженности в канале сбыта "Розница" на 15%;повышение до должности коммерческого директора.Начальник торгового отделасен 2010 - ноя 2014 (4 года 3 мес)Государственное предприятие"Чайка"FMCG
+				Обязанности:стратегическое планирование и развитие продаж;составление бюджетов продаж и расходов отдела;разработка мероприятий по увеличению объемов продаж;оперативное управление отделом: организация работы, координация, контроль выполнения плана продаж, составление отчетов.контроль дебиторской задолженности, работа с просроченной задолженностью;ведение переговоров с ключевыми клиентами и расширение клиентской базы; Достижения:привлечение к сотрудничеству национальных розничных сетей Auchan и Novus;увеличение объема продаж молочной продукции за счет подписание договора СТМ с сетью Караван;развитие фирменной розницы;заключение прямых договоров на поставку сырьевых товаров с крупными предприятиями FMCG сектора;Менеджер торгового отделаиюл 2009 - сен 2010 (1 год 3 мес)Государственное предприятие "Чайка"FMCG
+				консультация клиентов относительно продукции компании;работа с существующей клиентской базой;привлечение новых клиентов;ведение отчетности перед руководством.</t>
+        </is>
+      </c>
+      <c r="J232" t="inlineStr">
+        <is>
+          <t>Киевский национальный экономический университет имени Вадима Гетьмана(Киев, Украина)
+			Год окончания
+				2014
+			Финансово экономический факультет, Кандидат экономических наук
+		Киевский национальный университет имени Вадима Гетьмана(Киев, Украина)
+			Год окончания
+				2011
+			Факультет международной экономики, магистр
+			</t>
+        </is>
+      </c>
+      <c r="K232" t="inlineStr">
+        <is>
+          <t>Английский- выше среднего
+			Могу проходить собеседование на этом языкеФранцузский- базовый
+		</t>
+        </is>
+      </c>
+      <c r="L232" s="8" t="n">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Роберт</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>https://rabota.ua/cv/8275403</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Киев</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I233" t="inlineStr">
+        <is>
+          <t>
+Региональный менеджер FMCGокт 2006 - настоящее время (13 лет 3 мес)Bonduelle(http://bonduelle.ua/)
+				FMCG
+				Проведение переговоров с ключевыми клиентамиПланирование маркетингового бюджета, организация промо-мероприятияАнализ рынка и розницыПланирование продаж, работа с отчетностьюКонтроль продаж по региону, разработка мотивационных схем для дистрибьюторовРегиональный представительмай 2006 - окт 2006 (6 мес)Best sellerFMCG
+				Продвижение нового продукта с «нуля»; Поиск дистрибьюторов, заключение договоров; Организация и контроль продаж; Работа с командой дистрибьютора (обучение, мотивирование и т.д.)Планирование продаж и работа с отчетностью.Супервайзерсен 2002 - май 2006 (3 года 9 мес)Wrigley Ukraine(http://www.wrigley.com)
+				от 100 до 250 сотрудников
+					FMCG
+				Координация и контроль работы торговых представителей и мерчандайзеров; Организация и контроль продаж; Проведение переговоров с новыми клиентами; Организация размещения рекламы; Разработка рекламного и торгового оборудования;Проведение сторчеков, тренингов и митингов для торговых представителей и мерчандайзеров;Менеджер по закупкаммай 2001 - авг 2002 (1 год 4 мес)Золотой Востокот 100 до 250 сотрудников
+					Другое
+				Организация обеспечения компании (транспортный отдел, производственный отдел); Поиск поставщиков; Ведение переговоров об оптовых поставках; Закупка материала;Отслеживание остатков на складе.</t>
+        </is>
+      </c>
+      <c r="J233" t="inlineStr">
+        <is>
+          <t>Полтавский национальный технический университет(Полтава, Украина)
+			Год окончания
+				2014
+			Промышленное гражданское строительство, Бакалавр
+		Харьковский университет внутренних дел(Харьков, Украина)
+			Год окончания
+				1999
+			Правоведение. Юрист, Магистр
+			</t>
+        </is>
+      </c>
+      <c r="L233" s="8" t="n">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Дмитрий</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>https://rabota.ua/cv/7617323</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>Киев</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I234" t="inlineStr">
+        <is>
+          <t>
+Региональный менеджер по продажам (Киевская, Чернигоаская, Черкасская, Винницкая, Житомирская обл)фев 2013 - фев 2015 (2 года 1 мес)ООО «Колгейт Палмолив Украина» FMCG
+				Территоримальный менеджер по продажамфев 2004 - фев 2013 (9 лет 1 мес)ООО « Проктер енд Гембл Трейдинг Украина»FMCG
+				</t>
+        </is>
+      </c>
+      <c r="K234" t="inlineStr">
+        <is>
+          <t>Английский- средний
+		</t>
+        </is>
+      </c>
+      <c r="L234" s="8" t="n">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Лариса Александровна</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>https://rabota.ua/cv/9180222</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>Одесса</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>50000</t>
+        </is>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>Достижения: создание компании ООО «Донецк-Агропродукт», ООО «Доннафтасервис» с нуля.Осуществление бизнес-проекта : Строительство завода по переработке сельхозпродукции (зерновых, кукурузы, подсолнечника,сои) по гос. иновационно-инвестиционной программе при Министерстве экономики Украины.2009 г.Навыки: Бухучет, аудит, товароведение, технология производства пищевых продуктов,непродовольственных товаров, маркетинг, коммерческие продажи.Организация работы цепи поставок.   Разработка и осуществление участия предприятия в государственных и коммерческих тендерах.           </t>
+        </is>
+      </c>
+      <c r="I235" t="inlineStr">
+        <is>
+          <t>
+Директор ДП"Агролайт", директор ООО"Малка-транс" в корпорации Милкилэнд-Украина сен 2013 - настоящее время (6 лет 4 мес)Корпорация Милкилэнд-Украина, ДП «Агролайт»( Молочный комбинат, 675 сотрудников, г.Кривой рог)FMCG
+				контроль бюджетного планированияконтроль действия всех структурных подразделений, цехов и участков, тактическое стратегическое управление заводами . Конкретно:организация и контроль работы непосредственно производственников на обьектахорганизация и контроль по обеспечению бесперебойного поступления на заводы сырья для производства продукцииразработка стратегии компании на годовой период , с последующими корректировками ежеквартальноуправление отделом продаж, с ежемесячной постановкой и контролем выполнения планов продаж.проведение переговоров с бизнес-партнерами.взаимодействия с органами властиведение совместно с бухгалтерией финансового учета предприятия (ежемесячный анализ отчета о прибылях и убытках, баланс,ведения платежных календарей.контроль дебиторской задолженностизаключение договоровГенеральный  директор г. Киев,Одесса.янв 2010 - окт 2013 (3 года 10 мес)ООО «УК Мега-групп»Недвижимость и Девелопмент
+				Управление работой фирмы Контроль координация фиансового, налогового, управленческого учета  Анализ финансово-хозяйственной деятельности Контроль бюджетного планированияКоммерческий директор г. Донецкиюл 2004 - янв 2010 (5 лет 7 мес)ООО «Донецк-Агропродукт»АПК (Агропромышленный комплекс)
+				Управление работой фирмыОрганизация финансового, налогового и управленческого учетаУчет импортных операцийКоординация работ по проведению анализа финансово-хозяйственной деятельности, управление движением финансовых ресурсов, контроль бюджетного планированияРазвитие программы «Сельское хозяйство», коммерческая деятельность с сельхозпроизводителями, экспорт зерна, кукурузы, подсолечника и все что с этим связано. Полный комплекс работ от подготовкие договоров , работы с таможней,железной дорогой, с органами государственной властиРазработка и внедрение проекта льготного кредитования фирмы на пополнение оборотных средств и закупку основных фондовРазвитие сети продаж продукции сельского хозяйства, составление сметы производственных затратРазработка бизнес проекта «Строительство завода по переработке семян подсолнечника по государственной инновационно-инвестиционной программе»,регистрация проекта в центре экспертиз инноваций при Министерстве науки и образования, в Министерстве аграрной политики, Министерстве экономики, Мин. финансов, в органах исполнительной власти и гос. казначействеКоммерческий директор г. Донецкавг 1994 - окт 2004 (10 лет 3 мес)ООО «Доннафтасервис»Энергетика и Энергоносители
+				Покупка и продажа нефтепродуктов оптом и в розницуРазработка и внедрение бизнес проектов «Нефтеюганск-Линос» (ЛПНЗ)Работа с векселямиПолучение кредитов в банкахРазвитие клиентской базыРешение юридических вопросов</t>
+        </is>
+      </c>
+      <c r="J235" t="inlineStr">
+        <is>
+          <t>Донецкий Институт Советской Торговли (Донецк, Украина)
+			Год окончания
+				1991
+			Экономика и товароведение непродовольственных товаров, магистр
+		Докучаевский торговый техникум Министерства угольной промышленности СССР(Донецк)
+			Год окончания
+				1984
+			Товароведение промышленных товаров
+			</t>
+        </is>
+      </c>
+      <c r="K235" t="inlineStr">
+        <is>
+          <t>Английский- средний
+		Русский- родной
+			Могу проходить собеседование на этом языкеУкраинский- свободно
+			Могу проходить собеседование на этом языке</t>
+        </is>
+      </c>
+      <c r="L235" s="8" t="n">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Татьяна</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>https://rabota.ua/cv/9105056</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>Киев</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H236" t="inlineStr">
+        <is>
+          <t>Опыт создания и внедрения с «нуля» комплексной системы обучения и развития персонала отдела продаж (300 человек) в фармацевтической международной компании (Украина и СНГ).Профессионал разработки и проведения аудиторных тренингов и дистанционного обучения. Провела более 450 тренингов (4000 ч).Отличные навыки оценки потребности в обучении, ежегодного планирования обучения, оценки эффективности обучения, формирования бюджета, кадрового резерва12 лет в продажах, 6 лет тренерского опыта</t>
+        </is>
+      </c>
+      <c r="I236" t="inlineStr">
+        <is>
+          <t>
+студентиюн 2015 - июл 2016 (1 год 2 мес)Lifelong Learning Center(http://missoulaclasses.com/)
+				от 20 до 50 сотрудников
+					Образование
+				ESL (English Second Language) - обучение в США. Skype - tatyana.sukonnikovaВозвращение в Украину - август. Руководитель сектора управленческого  обучения депаратмента продажапр 2013 - июн 2015 (2 года 3 мес)АРТЕРІУМ / ARTERIUM(http://www.arterium.ua)
+				более 500 сотрудников
+					Фармацевтика
+				Обязанности:  Стратегическое планирование деятельности корпоративного обучения департамента продаж (300 человек). Выявление потребности в обучении и формирование целевых групп для обучения. Оценка эффективности обучения, участие в формировании кадрового резерва. ОтчетностьУправление бюджетом обучения коммерческого департамента. Взаимодействие с внешними поставщиками обучения. Разработка и внедрение долгосрочных и краткосрочных программ обучения и развития сотрудников отдела продаж согласно стандартам компании, намеченным целям. Проведение тренингов для управленцев среднего звена, линейного менеджмента, линейного персонала. Проведение дистанционного обучения (скайп-конференции, вебинары, онлайн-обучение). Мониторинг рынка методов обучения, поиск и оценка тренинговых продуктовПост-тренинговое сопровождение, коучинг. Сопровождение цикловых митингов. Наиболее значимые достижения: Разработана система «Книга знаний», объединяющая ошибки сотрудников и опыт преодоления их с последующей выработкой алгоритма предупреждения ошибок. Цель - снижение материальных затрат Корпорации.Внедрены ежемесячные факультативные мастер-классы по «Стрессменеджменту». Цель - повысить производительность труда сотрудников, улучшить психологический климат в коллективе.Проведено 170 тренингов для сотрудников коммерческого департамента в Украине, Белоруссии, Казахстане, УзбекистанеПортфель разработанных и приводящихся тренингов: · "Структура эффективного визита при работе с врачом, аптекой", "Коммуникация на визите с учетом психотипа собеседника", "Барьеры коммуникации и пути их преодоления", "Построение долгосрочных партнерских отношений с клиентом", "Взаимодействие со сложными клиентами", "Профессиональные навыки управления людьми", "Управление конфликтами в организации", " Профессиональные навыки рекрутинга", "Мотивация и управление командой", "Стресс и его профилактика", Командообразующие тренинги под потребности заказчика ( от 6 до 100 человек) с обратной связью руководителю.Рекомендации
+					Коростелева Ольга
+								Руководитель отдела обучения и развития ПАТ Киевмедпрепарат 
+								 Фармацевтическая  Корпорация «Артериум». 
+							по требованию
+							Юлия Сатыренко
+								Руководитель службы маркетинговых коммуникаций 
+								 Фармацевтическая  Корпорация «Артериум». 
+							по требованию
+							Тренинг – менеджер коммерческого департамента      май 2009 - апр 2013 (4 года)АРТЕРІУМ / ARTERIUM(http://www.arterium.ua)
+				более 500 сотрудников
+					Фармацевтика
+				Обязанности:Разработка и проведение тренингов для управленцев среднего звена, линейного менеджмента, линейного персонала коммерческого департамента в Украине, Казахстане, Узбекистане, Белоруссии, России. Управление бюджетом обучения коммерческого департамента. Планирование обучения. Взаимодействие с внешними поставщиками обучения. Оценка эффективности обучения, участие в формировании кадрового резерва.Координация бизнес-программ: до- и пост-тренинговое сопровождение. Коучинг-сесии с медицинскими представителями, региональными менеджерами, филдфорс менеджерами. Сопровождение цикловых митингов, модерация отработки проведения визитов.Ключевые достижения:Разработана и внедрена с " нуля" ступенчатая система обучения сотрудников отдела продаж.  Проведено более 250 тренингов.Создание и внедрение долгосрочного внутреннего обучения - школы Продакт-менеджеров и Региональных менеджеров для Медицинских представителейРекомендации
+					Волошина Татьяна
+								HR-менеджер 
+								Фармацевтическая Корпорация "Артериум"
+							(093)5918404
+							Региональный менеджер Центрального региона Rx  группымай 2007 - авг 2009 (2 года 4 мес)Фармацевтическая Корпорация "Артериум"(http://www.arterium.ua/en/)
+				более 500 сотрудников
+					Медицина и Здравоохранение
+				Обязанности: Достижения плановых показателей продаж в регионе.Организация работы региональной команды медицинских представителей. Подбор и обучение персонала (медицинские представители). Контроль проведения плановых визитов и отчетности МП. Ведение коммерческих переговоров с ключевыми клиентамиВедение планово-отчетной и рабочей документации. Организация и проведение презентаций, конференций, круглых столов.Ключевые достижения: Создание сильной команды профессионалов (9 МП) . При старте 3 МП. Отсутствие текучки кадров за 2008-2009г.Достижение командой плана продаж 108-110% в городах Черкассы и Житомир и 102-103% в Киеве 2008 - 2009 гг.Рекомендации
+					Калинская Алена
+								Руководитель кардио-гастро-неврологической службы 
+								Фармацевтическая Корпорация "Артериум"
+							(050)4468969
+							Медицинский представительфев 2003 - май 2007 (4 года 4 мес)Санофи Украина / Sanofi Ukraine(http://www.sanofi-aventis.com.ua/live/ua/ru/index.jsp)
+				более 500 сотрудников
+					Фармацевтика
+				Обязанности: выполнение плана продаж в в городах Киев, Бровары, Белая Церковь. Еженедельная отчетность. Семейный врачфев 2002 - мар 2003 (1 год 2 мес)Семейный доктор, Медицинский центр (http://www.family-doctor.kiev.ua)
+				от 20 до 50 сотрудников
+					Медицина и Здравоохранение
+				Лікар-терапевтавг 2001 - авг 2002 (1 год 1 мес)ТМО Жовтневого районаот 100 до 250 сотрудников
+					Медицина и Здравоохранение
+				</t>
+        </is>
+      </c>
+      <c r="J236" t="inlineStr">
+        <is>
+          <t>Киевский Государственный Медицинский Университет им. О.О. Богомольца (Киев, Украина)
+			Год окончания
+				2000
+			Лечебное дело, магистр
+		Киевский Государственный Педагогический  Университет им. Драгоманова(Киев, Украина)
+			Год окончания
+				1998
+			Природо-географический, магистр
+			</t>
+        </is>
+      </c>
+      <c r="K236" t="inlineStr">
+        <is>
+          <t>Английский- продвинутый
+			Могу проходить собеседование на этом языке</t>
+        </is>
+      </c>
+      <c r="L236" s="8" t="n">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Ашот Диасович</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>https://rabota.ua/cv/7624428</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>Киев</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G237" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="H237" t="inlineStr">
+        <is>
+          <t> Профессиональная деятельность: 2011-2016."Дерекція БШ-ТС м.Києва "інженер виробничого відділу будівництва ПМП.(согласование разрешений КиевБлагоустрий, Кабельные сети, Горадминистрация.2008-2010 «Генератор»(Климат) (Київ) Региональный менеджер   2006-2008-ООО «ЛПРЕС» (Дніпропетровськ) Коммерческий директор.(FMCG, Мебель.)  Организация и управление сбытом. Достижение высоких показателей по продажам.</t>
+        </is>
+      </c>
+      <c r="I237" t="inlineStr">
+        <is>
+          <t>
+Комм.Дпректор, Рнгиональн. Управляющийокт 2003 - дек 2008 (5 лет 3 мес)2006-08«ЛПРЕС» (Дніп-ськ)2003-2006 - ООО НПП "ЛВС" (Дніпропетровськ) от 20 до 50 сотрудников
+					FMCG
+				2006.08-2008.12«ЛПРЕС» (Дніпропетровськ) Коммерческий директор.(FMCG, Мебель.)Организация и управление сбытом. Построение и реализация системы продаж, снабжением. Контроль и управление розницей, оптом. Поиск новых дилеров ,переговоры, разработка условий для заключения договоров. Установление и развитие отношений с ключевыми клиентами. Разработка стратегических и перспективных планов развития. Разработка и реализация маркетинговых программ, системы закупок, ценообразования, маркетинг тенденций, Ценовая политика Участие в рекламных проектах (выставки, пресса, полиграфия). Достижение высоких показателей по продажам. 2003-2006 - ООО НПП "ЛВС" (Дніпропетровськ) Управляющий в Киевском регионе.(FMCG,Мебель)                                                                                                                                         Организация и управление сбытом, поиск новых дилеров, заключение и ведение договоров. Достижение объемов продаж продукции компании на вверенной территории. Разработка и согласование новых форм сотрудничества с дилерами. Весь спектр работ по представлению фирмы в регионе. Стратегическое и перспективное планирование по развитию региона. Маркетинг тенденций мебельного рынка, мебельных тканей и комплектующих. Ценовая политика меб. Рынка. Контроль заказов(производство, отгрузка, рекламации, дебиторка), Участие в выставках. Достижение рекордных показателей региона.1997.09-2001.02 ООО "Арлан", ООО "Арлан-мет" Пром.группа.(г.Москва) Заместитель директора по развитию фирмы (филиала г. Запорожье) заключение и ведение контрактов, разработка новых направлений п\п,тнп. Алюминиевые сплавы, цвет мет, чёрн. металл, чугун, ферросплавы, сырьё неопход. для производства в металлургии и машиностроении. Стратегическое и оперативное планирование бизнеса на территории Украины. Вывод филиала на самостоятельность и прибыльность.1995.07-1997.08 ООО "Геснерия-Центр" (Днепропетровск) Директор филиала фирмы в г.Харьков. (прод. питание) Весь Объём работ по представлению фирмы в регионе. Детское питание (пюре, сухие и молочные смеси, детские товары и игрушки. (офис, склад, контроль учета, отчетность перед головным офисом, контроль дебиторской задолженности.) Подъём филиала из завала на уровень
+			</t>
+        </is>
+      </c>
+      <c r="J237" t="inlineStr">
+        <is>
+          <t>2001-окончил Тернопольскую Академию народного хозяйства (г. Тернополь)1993-окончил Днепропетровский институт инженеров транспорта (г.Днепропетровск)(Днепропетровск, Тернополь)
+			Год окончания
+				2011
+			Факультет: Механический Квалификация: инженер-механик,Факультет: Финансы Квалификация: экономист, Специалист,Специалист.
+		Днепропетровский институт инженеров транспорта(Днепропетровск)
+			Год окончания
+				1993
+			Механический, Инженер/вагонное х-во,вагоностоение  
+			</t>
+        </is>
+      </c>
+      <c r="L237" s="8" t="n">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Дмитрий Сергеевич</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>https://rabota.ua/cv/10102187</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>Донецк</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I238" t="inlineStr">
+        <is>
+          <t>
+Директориюл 2015 - настоящее время (4 года 6 мес)ООО «Росагро»FMCG
+				Обязанности  Организация и контроль системной и эффективной работы, обеспечение выполнения задач по принятым проектам:   Личные достижения:Развитее с нуля импортного бизнеса компанииПодбор и обучение персоналаУвеличение клиентской базыРазработка и воплощение стратегии (50% от объема закупок по предоплате,  50% по факту отгрузки)Стремительный рост продаж      Мотив смены работы:  собственником принято решение о ликвидацииРекомендации
+					Дариенко Сергей Петрович 
+								Собственник 
+								ООО«Росагро»
+							(099)178-06-06
+							Дариенко Сергей Петрович 
+								Собственник 
+								ООО«Росагро»
+							(099)178-06-06
+							Дариенко Сергей Петрович 
+								Собственник 
+								ООО«Росагро»
+							(099)178-06-06
+							Дариенко Сергей Петрович 
+								Собственник 
+								ООО«Росагро»
+							(099)178-06-06
+							Директор по продажамянв 2012 - фев 2015 (3 года 2 мес)ООО «Донагротрейд»Торговля оптовая / Дистрибуция / Импорт-экспорт
+				Обязанности  Организация и контроль системной и эффективной работы команды, по закупкам и сбыту продукции агропромышленного комплекса   Личные достижения:100% Выполнение по объему продаж и фокусным задачам.Увеличения активной клиентской базы, а также ассортиментной линейки Компании-  Выход компании на экспортные продажи Мотив смены работы:  территориальная нестабильность, изменение законодательстваРекомендации
+					Быков Владимир Давыдович 
+								Соучередитель 
+								ООО «Донагротрейд»
+							0504227166
+							Быков Владимир Давыдович 
+								Соучередитель 
+								ООО «Донагротрейд»
+							0504227166
+							Быков Владимир Давыдович 
+								Соучередитель 
+								ООО «Донагротрейд»
+							0504227166
+							Быков Владимир Давыдович 
+								Соучередитель 
+								ООО «Донагротрейд»
+							0504227166
+							Быков Владимир Давыдович 
+								Соучередитель 
+								ООО «Донагротрейд»
+							0504227166
+							Быков Владимир Давыдович 
+								Соучередитель 
+								ООО «Донагротрейд»
+							0504227166
+							Быков Владимир Давыдович 
+								Соучередитель 
+								ООО «Донагротрейд»
+							0504227166
+							Быков Владимир Давыдович 
+								Соучередитель 
+								ООО «Донагротрейд»
+							0504227166
+							Начальник отдела продаж дек 2008 - ноя 2012 (4 года)ООО «ДИАД-АЗОВ»FMCG
+				Обязанности  Организация и контроль системной и эффективной работы команды по продажам, обеспечение выполнения задач по принятым проектам и ДЗ:Личные достижения:Подбор и обучение новой команды супервайзеров - увеличение качественной и количественной дистрибуции.Снижение на 80% просроченной дебиторской задолженностиВыполнение спецпроектов по представленности отдельных ТМ ;Изменение мотивации команд общего прайса - увеличение покрытия и рост продаж выделенных ТМ.Введение стандартов отчетности ТПМотив смены работы:  Собственное желаниеРекомендации
+					Бойко Иван Борисович 
+								Директор филиала 
+								«ДИАД-АЗОВ» 
+							(050)621-04-51
+							Бойко Иван Борисович 
+								Директор филиала 
+								«ДИАД-АЗОВ» 
+							(050)621-04-51
+							Начальник отдела продажфев 2011 - янв 2012 (1 год)ООО «ТД Доминион»FMCG
+				Обязанности  Контроль выполнения работ по поддержанию стандартов в сфере продаж и мерчандайзинга на рынке, для достижения доминирования над конкурентами (ТМ «Страйк» и ТМ «Марти Рей»)   Личные достижения:Подбор, обучение и контроль эксклюзивной команды СВ и ТП с нуля.100% выполнение ключевых показателейУвеличение объемов продаж продукции Компании, путем увеличения активной клиентской базы, а также качественной представленности в розницеПодготовка двух торговых агентов не должность супервайзер  Мотив смены работы: Продукция компании производителя ООО «Алкон+»  арестованаРекомендации
+					Мединский Федор Анатольевич 
+								Региональный менеджер 
+								ООО «Алкон +»               
+							(050)367-78-83
+							Мединский Федор Анатольевич 
+								Региональный менеджер 
+								ООО «Алкон +»               
+							(050)367-78-83
+							Мединский Федор Анатольевич 
+								Региональный менеджер 
+								ООО «Алкон +»               
+							(050)367-78-83
+							Территориальный менеджер по сбыту (ASM)авг 2007 - ноя 2008 (1 год 4 мес)ЗАО «Сармат»- «SAB MILLER» FMCG
+				Обязанности  Организация и контроль системной и эффективной работы областных команд дистрибуторов по продажам, обеспечение выполнения задач по принятым проектам.Личные достижения:Подбор новой команды супервайзеров - увеличение качественной и количественной дистрибуции.Ведение переговоров с потенциальными партнерами, подбор новых партнеров, обучение и контроль с момента запуска;Сокращение затратной части уже существующих партнеров (ремаршрутизация, веерная логистика, совместная логистика, создание и мотивация фокусных командВыполнение планов продажРазработка и подписание с дистрибутором графика выборки продукции - уменьшение нагрузки проплат дистрибутором ДЗМотив смены работы:  карьерный рост с изменением территории (Донецкая обл.)Рекомендации
+					Нехаев Алексей Валерьевич 
+								Региональный менеджер 
+								ЗАО «Сармат»- «SAB MILLER» 
+							(050)474-31-64
+							Нехаев Алексей Валерьевич 
+								Региональный менеджер 
+								ЗАО «Сармат»- «SAB MILLER» 
+							(050)474-31-64
+							Супервайзер FMCGсен 2006 - июн 2007 (10 мес)ЗАО «Сармат»FMCG
+				Обязанности  Контроль продаж и соблюдения ценовой политики  на закрепленной территории региона, развитие долгосрочных отношений с дистрибуторами. Контроль выполнения работ по поддержанию стандартов в сфере продаж и мерчандайзинга на рынке, для достижения доминирования над конкурентами:   Личные достижения:Подбор, обучение и контроль команды ЭТП.Увеличение объемов продаж продукции Компании, путем увеличения активной клиентской базы, а также качественной представленности в розницеРазмещение оборудования Компании, на стратегически важных для продажи местах, за счет перемещения и удаления оборудования конкурентов.  Мотив смены работы:  карьерный ростРекомендации
+					Нехаев Алексей Валерьевич 
+								Территориальный менеджер 
+								ЗАО «Сармат»
+							(050)474-31-64
+							Нехаев Алексей Валерьевич 
+								Территориальный менеджер 
+								ЗАО «Сармат»
+							(050)474-31-64
+							Торговый представительапр 2005 - сен 2006 (1 год 6 мес)Кока-Кола Бевериджис Лимитед Украина FMCG
+				Обязанности Обеспечение продаж и расширение дистрибуции ассортимента продукции,  размещение рекламных материалов, систематическое ведение отчетности и поточной документации по контролю за продажами.     Личные достижения:Увеличение объемов продаж продукции Компании, путем увеличения активной клиентской базы (с 170 РТТ до 250 РТТ), а также качественной представленности в рознице (увеличение представленности на основных и дополнительных местах продажи).-  Размещение оборудования Компании, на стратегически важных для продажи местах, за счет перемещения и удаления оборудования конкурентов.Мотив смены работы:  карьерный ростРекомендации
+					Яковенко Дмитрий Витальевич 
+								Территориальный менеджер 
+								Кока-Кола Бевериджис Лимитед Украина 
+							(050)387-32-06
+							</t>
+        </is>
+      </c>
+      <c r="J238" t="inlineStr">
+        <is>
+          <t>ДонНТУ (Менеджмент организаций)(Донецк)
+			Год окончания
+				2004
+			ФЭМ, Менеджмент организаций
+			</t>
+        </is>
+      </c>
+      <c r="K238" t="inlineStr">
+        <is>
+          <t>Английский- ниже среднего
+		</t>
+        </is>
+      </c>
+      <c r="L238" s="8" t="n">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Николай Николаевич</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>https://rabota.ua/cv/7835879</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>Херсон</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>Достигаю ощутимых результатов в работе над низко рентабельными проектами, эффективно справляюсь с задачами построения бизнеса с позиции start-up. При выполнении своих должностных обязанностей смотрю на решение поставленных задач под разными углами, порой с не стандартной стороны. Стремлюсь всегда выполнять поставленную задачу в короткие сроки с разумным использованием имеющихся ресурсов.На данный момент проживаю в Херсоне с желанием переехать в Киев, Львов, Одесса.</t>
+        </is>
+      </c>
+      <c r="I239" t="inlineStr">
+        <is>
+          <t>
+Директор коммерческийноя 2016 - настоящее время (3 года 2 мес)ООО "Экобиотек-Украина"Промышленность и Производство
+				Функциональные обязанности: Полный контроль коммерческого департамента предприятия;Формирование качественной базы поставщиков сырья и комплектующих;Контроль работы экспорта продукции и отдела продаж;Формирование цен на экспортируемую продукцию и на продукцию внутреннего рынка;Контроль заключения экспортных контрактов (с личным участием и контролем работы менеджеров по подписанию);Контроль отгрузок;Выбор экспедиторских и логистических компаний;Контроль использования эффективных фрахтовых ставок менеджерами;Заключение договоров логистики, снабжения, поставок комплектующих;Контроль работы логистики предприятия; Достижения: - Наладил эффективные взаимоотношения подотчётных отделов внутри департамента (снабжение, логистика, продажи);- Наладил эффективное сотрудничество между департаментами предприятия (коммерческого, бухгалтерского, производственного, складского и т. д);- Наладил ранее утерянные контакты и взаимоотношения с поставщиками;- Вернул в активную клиентскую базу тех, кто по разным причинам прекратил сотрудничество с предприятием;- Делегировал качественное распределение обязанностей и выполнение задач между подчинёнными;- Увеличил показатели эффективности снабжения сырьём и продажи готовой продукции.Менеджер ВЭДавг 2015 - ноя 2016 (1 год 4 мес)Хорольский молочно-консервный комбинат детских продуктов, ПАО(http://www.malysh.ua)
+				от 250 до 500 сотрудников
+					FMCG
+				Организация эффективных схем экспорта продукции компании и поиск новых рынков сбытаДиректор двух филиалов (Симферополь и Севастополь)янв 2011 - июн 2015 (4 года 6 мес)ДК "Европродукт"(http://europroduct.com.ua)
+				более 500 сотрудников
+					FMCG
+				Функциональные обязанности:- Контроль работы двух филиалов (Симферопольский и Севастопольский);- Организация и контроль работы всех структурных звеньев и сотрудников (38 человек) обоих филиалов;- Активное сотрудничество с Российскими поставщиками по прямым контрактам;- Анализ коммерческих предложений Европейских и Российских поставщиков с последующим заключением договоров сотрудничества по наиболее выгодным предложениям;- Улучшение коммерческих условий сотрудничества с работающими поставщиками и поиск новых;- Выполнение функций коммерческого директора на вверенных филиалах (переговоры с поставщиками, выбор и налаживание отношений с наиболее перспективными из них, установка реализационных цен с учётом изменяющейся конъюнктуры рынка);- Выполнение функций финансового руководителя филиалов (составление бюджета на месяц, квартал, год). Контроль расходования товарно-материальных ценностей, поиск и оптимизация возможностей экономии ежемесячных расходов филиалами;- Построение логистической системы работы своих и привлечённых автомобилей доставки;- Контроль работы отдела бухгалтерии и кассы;- Систематический контроль обеспечения филиалов эффективным товарным запасом, организация слаженной и рентабельной работы службы логистики (5 автомобилей доставки и 5 маршрутов ежедневно);- Обучение и поддержка торговой команды на филиалах (12 человек);- Участие в тендерах и проведение ежемесячных региональных собраний с привлечением сотрудников всех уровней на вверенной территории;- Организация и проведение переговоров с представителями поставщиков, производителей и региональных менеджеров;- Контроль эффективного расходования денежных средств во всех сферах хозяйствования филиалов и подразделений; - Контроль разделённых сфер функционирования филиалов не зависимо друг от друга: административно-управленческой, торговой (торговых представителей, супервайзеров, территориальных менеджеров, мерчендайзеров, менеджеров-операторов), логистической и складской (персонал склада и служба доставки).   Достижения:Осуществил полный и глубокий анализ рынка продуктов детского сегмента в АР Крым (декабрь 2010 г - январь 2011 г.) на этапе планирования и построения бизнес-плана организации филиалов в Симферополе и Севастополе. Организовал и наладил сотрудничество с Российскими поставщиками напрямую без включения в процесс главного офиса в связи с отсутствием, в дальнейшем, получения товара из Украины. Оптимизировал в течении 2014 года коммерческие условия поставки продукции от Российских и Европейских поставщиков, снизив себестоимость входящей продукции на 3 % в целом; Наладил оптимальную схему импортных поставок продукции с учётом влияния внешних факторов на графики поставок (в частности влияние на качество поставок перебойной работы Керченской переправы). Организовал бесперебойные поставки продукции на склад филиала от импортёров напрямую. Заключил ряд соглашений с импортёрами наСупервайзерсен 2010 - янв 2011 (5 мес)ЧП Сокульский Н. В.от 20 до 50 сотрудников
+					FMCG
+				Функциональные обязанности:  - Подбор торговых представителей и мерчандайзеров, проведение собеседований; - Внедрение в работу собственных разработок в сфере изменение политики взаимоотношений с каждой торговой точкой относительно возврата денежных средств и ускорения оборачиваемости средств; - Разработка и внедрение новых стандартов представленности «ведущего» (наиболее маржинального) ассортимента в разрезе всех сегментов и каналов сбыта; - Планирование продаж на вверенной территории; - Организация обучающих аспектов развития подотчётных сотрудников, организация и проведение собраний; - Систематический контроль функционирования (работы) торговой команды; - Отслеживание тенденций изменения рынка детских товаров и деятельности конкурентов; - Выведение на рынок новых брендов; - Разработка стратегии, проведение годовых переговоров с ключевыми торговыми сетями; - Разработка и контроль над исполнением комплекса маркетинговых мероприятий;  Достижения:Разработал и ввёл в действие программу новых приёмов бонусных мотиваций торговых представителей, увеличил показатель качественной дистрибьюции в оптовом канале на 11 %, в розничном канале системы «КЭШ and КЭРРИ» на 8 %, в канале специализированной розницы на 9 %. Изменил маршруты доставки, используя исключительно собственный транспорт логистики (находящийся в собственности ЧП Сокульский Н. В.) без аренды наёмного.  Принял на работу двух новых торговых представителей, обучил их основным моментам в работе и скоординировал дальнейшие шаги обеспечения качественной работы.</t>
+        </is>
+      </c>
+      <c r="J239" t="inlineStr">
+        <is>
+          <t>Симферопольский Юридический Институт филиал Харьковской Национальной Юридической Академии Украины им. Ярослава Мудрого.(Симферополь, АРК Крым)
+			Год окончания
+				2014
+			юриспруденция, бакалавр
+		Херсонский Государственный Аграрный Университет(Херсон, Украина)
+			Год окончания
+				2002
+			Менеджер-экономист, экономический факультет, бакалавр, специалист (красные дипломы)
+			</t>
+        </is>
+      </c>
+      <c r="K239" t="inlineStr">
+        <is>
+          <t>Английский- средний
+		Русский- свободно
+			Могу проходить собеседование на этом языкеУкраинский- родной
+			Могу проходить собеседование на этом языке</t>
+        </is>
+      </c>
+      <c r="L239" s="8" t="n">
+        <v>43804</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>